<commit_message>
Changed the way to save the XML file
</commit_message>
<xml_diff>
--- a/CONFIG/analyses.xlsx
+++ b/CONFIG/analyses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ECAR\OCR_ECAR\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766524D1-001E-40FA-B926-AEE6400772CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A805EC9-9042-42F2-866B-29D11C90D3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CU hors OAIC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="929">
   <si>
     <t>Quotation Version</t>
   </si>
@@ -2228,9 +2228,6 @@
     <t>PROTEINES DUMAS X 5.70 /SEC</t>
   </si>
   <si>
-    <t>Cyanures</t>
-  </si>
-  <si>
     <t>QF07P</t>
   </si>
   <si>
@@ -2249,9 +2246,6 @@
     <t>ZVR08</t>
   </si>
   <si>
-    <t>EUNLGR Service Rush TAT court (pesticides)</t>
-  </si>
-  <si>
     <t>Cyperméthrin</t>
   </si>
   <si>
@@ -2322,9 +2316,6 @@
   </si>
   <si>
     <t>QF01G</t>
-  </si>
-  <si>
-    <t>AFLATOXINES IMMUNO B1+B2+G1+G2</t>
   </si>
   <si>
     <t>QF0AD</t>
@@ -2730,9 +2721,6 @@
     <t>Ajout</t>
   </si>
   <si>
-    <t>DON Immuno QF01H</t>
-  </si>
-  <si>
     <t>EVERYTIME</t>
   </si>
   <si>
@@ -2778,9 +2766,6 @@
     <t>Pack Protéines Dumas sec x5,7 + Humidité</t>
   </si>
   <si>
-    <t>Ochratoxines A Immuno</t>
-  </si>
-  <si>
     <t>Pack sur sec x5,7 (incluant humidité) DUMAS</t>
   </si>
   <si>
@@ -2808,18 +2793,12 @@
     <t>Sanitaire</t>
   </si>
   <si>
-    <t>Zéaralénone Immuno QF01I</t>
-  </si>
-  <si>
     <t>Insectes vivants QF045</t>
   </si>
   <si>
     <t>Alvéogramme (QF001 +  A7500)</t>
   </si>
   <si>
-    <t>radioactivité</t>
-  </si>
-  <si>
     <t>Humidité uniquement (AA07A)</t>
   </si>
   <si>
@@ -2835,10 +2814,25 @@
     <t>ONE : SF00B AA239 AA23C AA20I</t>
   </si>
   <si>
-    <t>PTEST</t>
-  </si>
-  <si>
-    <t>P0000</t>
+    <t>AFLATOXINES IMMUNO B1+B2+G1+G2 (QF0AD)</t>
+  </si>
+  <si>
+    <t>OCHRATOXINES A IMMUNO (QF01G)</t>
+  </si>
+  <si>
+    <t>DON (Vomitoxines) Immuno (QF01H)</t>
+  </si>
+  <si>
+    <t>Tilletia indicia et controcersa (QF073)</t>
+  </si>
+  <si>
+    <t>Cyanures (QF07P)</t>
+  </si>
+  <si>
+    <t>Zéaralénone Immuno (QF01I)</t>
+  </si>
+  <si>
+    <t>Radioactivité (RR00L+RR00M+RRGAD)</t>
   </si>
 </sst>
 </file>
@@ -3104,7 +3098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3167,20 +3161,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3466,10 +3459,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E0E6888-AAC1-41FB-A141-E09E58FF398D}" name="Table1" displayName="Table1" ref="A1:F72" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A1:F72" xr:uid="{8E0E6888-AAC1-41FB-A141-E09E58FF398D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F71">
-    <sortCondition ref="E1:E71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E0E6888-AAC1-41FB-A141-E09E58FF398D}" name="Table1" displayName="Table1" ref="A1:F65" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A1:F65" xr:uid="{8E0E6888-AAC1-41FB-A141-E09E58FF398D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition ref="D1:D65"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A346BC8D-3196-4E82-9F55-180EB422D7AA}" name="Quotation Version" dataDxfId="5"/>
@@ -3768,10 +3761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3788,16 +3781,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="F1" s="38" t="s">
         <v>2</v>
@@ -3808,14 +3801,14 @@
         <v>716</v>
       </c>
       <c r="B2" s="26"/>
-      <c r="C2" s="53" t="s">
-        <v>924</v>
+      <c r="C2" s="51" t="s">
+        <v>917</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>717</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>718</v>
@@ -3826,17 +3819,17 @@
         <v>716</v>
       </c>
       <c r="B3" s="15"/>
-      <c r="C3" s="31" t="s">
-        <v>719</v>
+      <c r="C3" s="55" t="s">
+        <v>741</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>720</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>918</v>
+        <v>742</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>914</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>721</v>
+        <v>743</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -3844,17 +3837,17 @@
         <v>716</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="51" t="s">
-        <v>722</v>
+      <c r="C4" s="47" t="s">
+        <v>735</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>723</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>918</v>
+        <v>736</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>914</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -3862,17 +3855,17 @@
         <v>716</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="C5" s="31" t="s">
-        <v>719</v>
+      <c r="C5" s="47" t="s">
+        <v>738</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>918</v>
+        <v>739</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>914</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>726</v>
+        <v>740</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -3880,14 +3873,14 @@
         <v>716</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="31" t="s">
-        <v>912</v>
+      <c r="C6" s="50" t="s">
+        <v>907</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>206</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>727</v>
@@ -3898,229 +3891,233 @@
         <v>716</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="31" t="s">
-        <v>911</v>
+      <c r="C7" s="50" t="s">
+        <v>906</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>142</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="36" t="s">
         <v>716</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="30" t="s">
-        <v>774</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>775</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>776</v>
+      <c r="B8" s="18"/>
+      <c r="C8" s="47" t="s">
+        <v>799</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>513</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>914</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="36" t="s">
         <v>716</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="30" t="s">
-        <v>777</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>778</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>779</v>
+      <c r="B9" s="18"/>
+      <c r="C9" s="47" t="s">
+        <v>801</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>802</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>914</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="36" t="s">
         <v>716</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="48" t="s">
-        <v>926</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>780</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>781</v>
+      <c r="B10" s="18"/>
+      <c r="C10" s="47" t="s">
+        <v>804</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>805</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>914</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="36" t="s">
         <v>716</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="48" t="s">
-        <v>927</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>782</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>783</v>
+      <c r="B11" s="18"/>
+      <c r="C11" s="30" t="s">
+        <v>807</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>574</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="30" t="s">
-        <v>784</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>785</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>786</v>
+        <v>809</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>914</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>810</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>716</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="30" t="s">
-        <v>787</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>788</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>789</v>
+      <c r="B13" s="42"/>
+      <c r="C13" s="56" t="s">
+        <v>744</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>914</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A14" s="35" t="s">
         <v>716</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="52" t="s">
-        <v>922</v>
+      <c r="B14" s="20"/>
+      <c r="C14" s="30" t="s">
+        <v>814</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>793</v>
+        <v>568</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>792</v>
+        <v>769</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>716</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>574</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>918</v>
-      </c>
-      <c r="F15" s="18" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="47" t="s">
+        <v>928</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>767</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>914</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.45">
+      <c r="A16" s="35" t="s">
+        <v>716</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>897</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="20" t="s">
+        <v>821</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>914</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.45">
+      <c r="A17" s="36" t="s">
+        <v>716</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="30" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A16" s="34" t="s">
+      <c r="D17" s="18" t="s">
+        <v>812</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.45">
+      <c r="A18" s="35" t="s">
         <v>716</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="D16" s="15" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="47" t="s">
+        <v>916</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>790</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A17" s="34" t="s">
+      <c r="E18" s="8" t="s">
+        <v>913</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.45">
+      <c r="A19" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="50" t="s">
-        <v>921</v>
-      </c>
-      <c r="D17" s="46" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>825</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>914</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F17" s="41"/>
-    </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A18" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="44" t="s">
-        <v>915</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>916</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="F18" s="41"/>
-    </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A19" s="36" t="s">
-        <v>716</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="30" t="s">
-        <v>814</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>815</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>918</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>816</v>
+      <c r="F19" s="15" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4129,16 +4126,16 @@
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="30" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4147,34 +4144,34 @@
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="30" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="30" t="s">
-        <v>817</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>568</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>918</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>772</v>
+        <v>823</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4183,31 +4180,35 @@
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="30" t="s">
-        <v>729</v>
+        <v>774</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>730</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>919</v>
+        <v>775</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>913</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>731</v>
+        <v>776</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A24" s="54"/>
-      <c r="B24" s="4" t="s">
-        <v>928</v>
-      </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="4" t="s">
-        <v>735</v>
+      <c r="A24" s="34" t="s">
+        <v>716</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="31" t="s">
+        <v>719</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>725</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>736</v>
-      </c>
-      <c r="F24" s="4"/>
+        <v>913</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A25" s="34" t="s">
@@ -4215,16 +4216,16 @@
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="30" t="s">
-        <v>732</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>733</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>919</v>
+        <v>771</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>772</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>913</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>734</v>
+        <v>773</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4232,17 +4233,17 @@
         <v>716</v>
       </c>
       <c r="B26" s="15"/>
-      <c r="C26" s="30" t="s">
-        <v>737</v>
+      <c r="C26" s="47" t="s">
+        <v>923</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>738</v>
+        <v>758</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>739</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4250,17 +4251,17 @@
         <v>716</v>
       </c>
       <c r="B27" s="15"/>
-      <c r="C27" s="30" t="s">
-        <v>740</v>
+      <c r="C27" s="47" t="s">
+        <v>924</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>741</v>
+        <v>752</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>742</v>
+        <v>753</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4268,71 +4269,67 @@
         <v>716</v>
       </c>
       <c r="B28" s="15"/>
-      <c r="C28" s="45" t="s">
-        <v>743</v>
+      <c r="C28" s="47" t="s">
+        <v>927</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>919</v>
+        <v>749</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>914</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="31" t="s">
-        <v>746</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>435</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>919</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>747</v>
-      </c>
+      <c r="B29" s="41"/>
+      <c r="C29" s="44" t="s">
+        <v>910</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>911</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="F29" s="41"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A30" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="30" t="s">
-        <v>750</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>751</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>919</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>752</v>
-      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="49" t="s">
+        <v>915</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>909</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="F30" s="41"/>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A31" s="34" t="s">
         <v>716</v>
       </c>
       <c r="B31" s="15"/>
-      <c r="C31" s="30" t="s">
-        <v>753</v>
+      <c r="C31" s="47" t="s">
+        <v>919</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>754</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>919</v>
+        <v>777</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>913</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>755</v>
+        <v>778</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4340,17 +4337,17 @@
         <v>716</v>
       </c>
       <c r="B32" s="15"/>
-      <c r="C32" s="48" t="s">
-        <v>925</v>
+      <c r="C32" s="47" t="s">
+        <v>920</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>757</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>919</v>
+        <v>779</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>913</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>758</v>
+        <v>780</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4359,16 +4356,16 @@
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="30" t="s">
-        <v>759</v>
+        <v>788</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>760</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>919</v>
+        <v>787</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>913</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>129</v>
+        <v>788</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4377,16 +4374,16 @@
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="30" t="s">
-        <v>761</v>
+        <v>784</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>762</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>919</v>
+        <v>785</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>913</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>763</v>
+        <v>786</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4394,17 +4391,17 @@
         <v>716</v>
       </c>
       <c r="B35" s="15"/>
-      <c r="C35" s="30" t="s">
-        <v>767</v>
+      <c r="C35" s="47" t="s">
+        <v>925</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>768</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>919</v>
+        <v>782</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>913</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>769</v>
+        <v>783</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4412,125 +4409,125 @@
         <v>716</v>
       </c>
       <c r="B36" s="15"/>
-      <c r="C36" s="30" t="s">
-        <v>767</v>
+      <c r="C36" s="47" t="s">
+        <v>926</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>748</v>
+        <v>729</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>749</v>
+        <v>730</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="48" t="s">
-        <v>923</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>770</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>919</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>771</v>
+      <c r="B37" s="15"/>
+      <c r="C37" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>851</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B38" s="18"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="30" t="s">
-        <v>802</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>513</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>919</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>803</v>
+        <v>852</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>853</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="30" t="s">
-        <v>804</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>805</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>919</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>806</v>
+      <c r="B39" s="15"/>
+      <c r="C39" s="31" t="s">
+        <v>719</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>720</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="30" t="s">
-        <v>807</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>808</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>919</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>809</v>
+      <c r="B40" s="15"/>
+      <c r="C40" s="47" t="s">
+        <v>922</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>759</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>914</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="30" t="s">
-        <v>812</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>919</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>813</v>
+      <c r="B41" s="15"/>
+      <c r="C41" s="47" t="s">
+        <v>918</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>914</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B42" s="20" t="s">
-        <v>901</v>
-      </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="20" t="s">
-        <v>824</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>919</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>825</v>
+      <c r="B42" s="15"/>
+      <c r="C42" s="50" t="s">
+        <v>722</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>723</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4539,16 +4536,16 @@
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="30" t="s">
-        <v>910</v>
+        <v>854</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>760</v>
+        <v>855</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>129</v>
+        <v>854</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4557,16 +4554,16 @@
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="30" t="s">
-        <v>894</v>
+        <v>856</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>754</v>
+        <v>857</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>755</v>
+        <v>856</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4574,17 +4571,17 @@
         <v>716</v>
       </c>
       <c r="B45" s="15"/>
-      <c r="C45" s="48" t="s">
-        <v>920</v>
+      <c r="C45" s="30" t="s">
+        <v>834</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>751</v>
+        <v>835</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>752</v>
+        <v>836</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4593,16 +4590,16 @@
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="30" t="s">
-        <v>826</v>
+        <v>844</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>12</v>
+        <v>845</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>13</v>
+        <v>844</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4611,16 +4608,16 @@
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="30" t="s">
-        <v>827</v>
+        <v>862</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>828</v>
+        <v>863</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>829</v>
+        <v>862</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4629,16 +4626,16 @@
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="30" t="s">
-        <v>830</v>
+        <v>842</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>831</v>
+        <v>843</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>832</v>
+        <v>842</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4647,16 +4644,16 @@
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="30" t="s">
-        <v>833</v>
+        <v>848</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>834</v>
+        <v>849</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>835</v>
+        <v>848</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4665,16 +4662,16 @@
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="30" t="s">
-        <v>794</v>
+        <v>840</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>795</v>
+        <v>841</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>794</v>
+        <v>840</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4683,16 +4680,16 @@
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="30" t="s">
-        <v>796</v>
+        <v>846</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>797</v>
+        <v>847</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>796</v>
+        <v>846</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4701,16 +4698,16 @@
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="30" t="s">
-        <v>798</v>
+        <v>858</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>799</v>
+        <v>859</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>798</v>
+        <v>858</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4719,16 +4716,16 @@
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="30" t="s">
-        <v>800</v>
+        <v>860</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>801</v>
+        <v>861</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>800</v>
+        <v>860</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4737,16 +4734,16 @@
       </c>
       <c r="B54" s="15"/>
       <c r="C54" s="30" t="s">
-        <v>786</v>
+        <v>797</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>785</v>
+        <v>798</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>786</v>
+        <v>797</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4755,16 +4752,16 @@
       </c>
       <c r="B55" s="15"/>
       <c r="C55" s="30" t="s">
-        <v>843</v>
+        <v>793</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>844</v>
+        <v>794</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>843</v>
+        <v>793</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4773,16 +4770,16 @@
       </c>
       <c r="B56" s="15"/>
       <c r="C56" s="30" t="s">
-        <v>845</v>
+        <v>793</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>846</v>
+        <v>794</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>845</v>
+        <v>793</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4791,16 +4788,16 @@
       </c>
       <c r="B57" s="15"/>
       <c r="C57" s="30" t="s">
-        <v>847</v>
+        <v>791</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>848</v>
+        <v>792</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>847</v>
+        <v>791</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4809,16 +4806,16 @@
       </c>
       <c r="B58" s="15"/>
       <c r="C58" s="30" t="s">
-        <v>849</v>
+        <v>791</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>850</v>
+        <v>792</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>849</v>
+        <v>791</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4827,16 +4824,16 @@
       </c>
       <c r="B59" s="15"/>
       <c r="C59" s="30" t="s">
-        <v>851</v>
+        <v>795</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>852</v>
+        <v>796</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>851</v>
+        <v>795</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4845,16 +4842,16 @@
       </c>
       <c r="B60" s="15"/>
       <c r="C60" s="30" t="s">
-        <v>853</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>854</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>919</v>
+        <v>731</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>914</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>853</v>
+        <v>733</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4863,16 +4860,16 @@
       </c>
       <c r="B61" s="15"/>
       <c r="C61" s="30" t="s">
-        <v>855</v>
+        <v>764</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>856</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>919</v>
+        <v>765</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>914</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>855</v>
+        <v>766</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.45">
@@ -4881,189 +4878,67 @@
       </c>
       <c r="B62" s="15"/>
       <c r="C62" s="30" t="s">
-        <v>857</v>
+        <v>764</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>858</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>919</v>
+        <v>746</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>914</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>857</v>
+        <v>747</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A63" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="30" t="s">
-        <v>859</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>860</v>
+      <c r="B63" s="26"/>
+      <c r="C63" s="43" t="s">
+        <v>837</v>
+      </c>
+      <c r="D63" s="46" t="s">
+        <v>838</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>859</v>
+        <v>913</v>
+      </c>
+      <c r="F63" s="26" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A64" s="34" t="s">
         <v>716</v>
       </c>
-      <c r="B64" s="15"/>
-      <c r="C64" s="30" t="s">
-        <v>861</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>862</v>
+      <c r="B64" s="26" t="s">
+        <v>891</v>
+      </c>
+      <c r="C64" s="48"/>
+      <c r="D64" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F64" s="15" t="s">
-        <v>861</v>
+        <v>913</v>
+      </c>
+      <c r="F64" s="26" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A65" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B65" s="15"/>
-      <c r="C65" s="30" t="s">
-        <v>863</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>864</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A66" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B66" s="15"/>
-      <c r="C66" s="30" t="s">
-        <v>865</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>866</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F66" s="15" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A67" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B67" s="15"/>
-      <c r="C67" s="30" t="s">
-        <v>794</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>795</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F67" s="15" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A68" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>797</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A69" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B69" s="15"/>
-      <c r="C69" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>799</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F69" s="15" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A70" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B70" s="26"/>
-      <c r="C70" s="43" t="s">
-        <v>800</v>
-      </c>
-      <c r="D70" s="47" t="s">
-        <v>801</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F70" s="26" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A71" s="34" t="s">
-        <v>716</v>
-      </c>
-      <c r="B71" s="26" t="s">
-        <v>895</v>
-      </c>
-      <c r="C71" s="49"/>
-      <c r="D71" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="E71" s="15"/>
-      <c r="F71" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A72" s="55"/>
-      <c r="B72" s="56"/>
-      <c r="C72" s="57" t="s">
-        <v>929</v>
-      </c>
-      <c r="D72" s="56" t="s">
-        <v>930</v>
-      </c>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
+      <c r="A65" s="52"/>
+      <c r="B65" s="53" t="s">
+        <v>921</v>
+      </c>
+      <c r="C65" s="54"/>
+      <c r="D65" s="53" t="s">
+        <v>734</v>
+      </c>
+      <c r="E65" s="53" t="s">
+        <v>914</v>
+      </c>
+      <c r="F65" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5078,8 +4953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1D9E95-6621-4612-B1CC-F9B119517B93}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5096,16 +4971,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -5113,35 +4988,35 @@
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="24" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="24" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>717</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>718</v>
@@ -5149,233 +5024,233 @@
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="24" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="24" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="24" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="25" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="25" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="25" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="23" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="23" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="25" t="s">
         <v>261</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="25" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="25" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="4" t="s">
         <v>116</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>117</v>
@@ -5383,17 +5258,17 @@
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="4" t="s">
         <v>110</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>111</v>
@@ -5401,35 +5276,35 @@
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="4" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="24" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>113</v>
@@ -5437,17 +5312,17 @@
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="19" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>124</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>125</v>
@@ -5455,17 +5330,17 @@
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="19" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>120</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>121</v>
@@ -5473,17 +5348,17 @@
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="19" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>118</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>119</v>
@@ -5491,53 +5366,53 @@
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="24" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="24" t="s">
+        <v>754</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>757</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="24" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>129</v>
@@ -5545,106 +5420,108 @@
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="24" t="s">
+        <v>751</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>753</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>754</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="24" t="s">
+        <v>748</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>750</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>751</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="25" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="25" t="s">
         <v>719</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="23" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>913</v>
+      </c>
       <c r="F31" s="4" t="s">
         <v>8</v>
       </c>
@@ -5676,10 +5553,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -5710,7 +5587,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="4" t="s">
@@ -5754,7 +5631,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="4" t="s">
@@ -5993,7 +5870,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="4" t="s">
@@ -7356,7 +7233,7 @@
         <v>4</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="C106" s="14"/>
       <c r="D106" s="4" t="s">
@@ -9152,7 +9029,7 @@
         <v>4</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="C216" s="17"/>
       <c r="D216" s="4" t="s">

</xml_diff>